<commit_message>
grouping and column split fixed hopefully
</commit_message>
<xml_diff>
--- a/BSDT-statistical-analysis/media/ID_36_uploads/temporary_uploads/Depression_Questionnaire_Responses.xlsx
+++ b/BSDT-statistical-analysis/media/ID_36_uploads/temporary_uploads/Depression_Questionnaire_Responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC61"/>
+  <dimension ref="A1:AH61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,6 +579,31 @@
           <t>PHQ9_Total</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Significant_Diseases_part_1</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Significant_Diseases_part_2</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Significant_Diseases_part_3</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Friends_To_Talk_part_1</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Friends_To_Talk_part_2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -706,6 +731,27 @@
       <c r="AC2" t="n">
         <v>14</v>
       </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>Chronic pain</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Cancer</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -833,6 +879,23 @@
       <c r="AC3" t="n">
         <v>13</v>
       </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -956,6 +1019,23 @@
       <c r="AC4" t="n">
         <v>13</v>
       </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>Neurological disorders</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1083,6 +1163,27 @@
       <c r="AC5" t="n">
         <v>12</v>
       </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>Thyroid problems</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diabetes</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1210,6 +1311,23 @@
       <c r="AC6" t="n">
         <v>7</v>
       </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1337,6 +1455,19 @@
       <c r="AC7" t="n">
         <v>9</v>
       </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1464,6 +1595,27 @@
       <c r="AC8" t="n">
         <v>15</v>
       </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>Thyroid problems</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Neurological disorders</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> None</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1591,6 +1743,23 @@
       <c r="AC9" t="n">
         <v>14</v>
       </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>Cancer</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1718,6 +1887,27 @@
       <c r="AC10" t="n">
         <v>5</v>
       </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>Cancer</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Stroke</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1845,6 +2035,23 @@
       <c r="AC11" t="n">
         <v>11</v>
       </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>Neurological disorders</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1972,6 +2179,31 @@
       <c r="AC12" t="n">
         <v>12</v>
       </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>High blood pressure</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diabetes</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Other</t>
+        </is>
+      </c>
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2099,6 +2331,27 @@
       <c r="AC13" t="n">
         <v>13</v>
       </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> None</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2226,6 +2479,23 @@
       <c r="AC14" t="n">
         <v>16</v>
       </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2353,6 +2623,23 @@
       <c r="AC15" t="n">
         <v>10</v>
       </c>
+      <c r="AD15" t="inlineStr"/>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Heart disease</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2480,6 +2767,23 @@
       <c r="AC16" t="n">
         <v>14</v>
       </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>Neurological disorders</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2607,6 +2911,23 @@
       <c r="AC17" t="n">
         <v>12</v>
       </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>Cancer</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2734,6 +3055,23 @@
       <c r="AC18" t="n">
         <v>8</v>
       </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>Diabetes</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2857,6 +3195,19 @@
       <c r="AC19" t="n">
         <v>12</v>
       </c>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2984,6 +3335,23 @@
       <c r="AC20" t="n">
         <v>9</v>
       </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>Chronic pain</t>
+        </is>
+      </c>
+      <c r="AE20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3111,6 +3479,23 @@
       <c r="AC21" t="n">
         <v>18</v>
       </c>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>Diabetes</t>
+        </is>
+      </c>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3238,6 +3623,27 @@
       <c r="AC22" t="n">
         <v>14</v>
       </c>
+      <c r="AD22" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Other</t>
+        </is>
+      </c>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3365,6 +3771,23 @@
       <c r="AC23" t="n">
         <v>16</v>
       </c>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
+      <c r="AE23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3492,6 +3915,27 @@
       <c r="AC24" t="n">
         <v>13</v>
       </c>
+      <c r="AD24" t="inlineStr">
+        <is>
+          <t>Diabetes</t>
+        </is>
+      </c>
+      <c r="AE24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> None</t>
+        </is>
+      </c>
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AG24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3619,6 +4063,19 @@
       <c r="AC25" t="n">
         <v>15</v>
       </c>
+      <c r="AD25" t="inlineStr">
+        <is>
+          <t>Cancer</t>
+        </is>
+      </c>
+      <c r="AE25" t="inlineStr"/>
+      <c r="AF25" t="inlineStr"/>
+      <c r="AG25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3746,6 +4203,23 @@
       <c r="AC26" t="n">
         <v>14</v>
       </c>
+      <c r="AD26" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="AE26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Heart disease</t>
+        </is>
+      </c>
+      <c r="AF26" t="inlineStr"/>
+      <c r="AG26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3873,6 +4347,31 @@
       <c r="AC27" t="n">
         <v>20</v>
       </c>
+      <c r="AD27" t="inlineStr">
+        <is>
+          <t>Thyroid problems</t>
+        </is>
+      </c>
+      <c r="AE27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AF27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Chronic pain</t>
+        </is>
+      </c>
+      <c r="AG27" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4000,6 +4499,19 @@
       <c r="AC28" t="n">
         <v>10</v>
       </c>
+      <c r="AD28" t="inlineStr">
+        <is>
+          <t>Chronic pain</t>
+        </is>
+      </c>
+      <c r="AE28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4127,6 +4639,31 @@
       <c r="AC29" t="n">
         <v>10</v>
       </c>
+      <c r="AD29" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
+      <c r="AE29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diabetes</t>
+        </is>
+      </c>
+      <c r="AF29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Stroke</t>
+        </is>
+      </c>
+      <c r="AG29" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4254,6 +4791,23 @@
       <c r="AC30" t="n">
         <v>9</v>
       </c>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Other</t>
+        </is>
+      </c>
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diabetes</t>
+        </is>
+      </c>
+      <c r="AG30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4381,6 +4935,27 @@
       <c r="AC31" t="n">
         <v>15</v>
       </c>
+      <c r="AD31" t="inlineStr">
+        <is>
+          <t>Diabetes</t>
+        </is>
+      </c>
+      <c r="AE31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thyroid problems</t>
+        </is>
+      </c>
+      <c r="AF31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Cancer</t>
+        </is>
+      </c>
+      <c r="AG31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4508,6 +5083,31 @@
       <c r="AC32" t="n">
         <v>9</v>
       </c>
+      <c r="AD32" t="inlineStr">
+        <is>
+          <t>Chronic pain</t>
+        </is>
+      </c>
+      <c r="AE32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Heart disease</t>
+        </is>
+      </c>
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> None</t>
+        </is>
+      </c>
+      <c r="AG32" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4635,6 +5235,27 @@
       <c r="AC33" t="n">
         <v>12</v>
       </c>
+      <c r="AD33" t="inlineStr">
+        <is>
+          <t>Diabetes</t>
+        </is>
+      </c>
+      <c r="AE33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AF33" t="inlineStr"/>
+      <c r="AG33" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4762,6 +5383,31 @@
       <c r="AC34" t="n">
         <v>17</v>
       </c>
+      <c r="AD34" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="AE34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Stroke</t>
+        </is>
+      </c>
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AG34" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4889,6 +5535,31 @@
       <c r="AC35" t="n">
         <v>9</v>
       </c>
+      <c r="AD35" t="inlineStr">
+        <is>
+          <t>Cancer</t>
+        </is>
+      </c>
+      <c r="AE35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diabetes</t>
+        </is>
+      </c>
+      <c r="AF35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Neurological disorders</t>
+        </is>
+      </c>
+      <c r="AG35" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -5012,6 +5683,15 @@
       <c r="AC36" t="n">
         <v>9</v>
       </c>
+      <c r="AD36" t="inlineStr"/>
+      <c r="AE36" t="inlineStr"/>
+      <c r="AF36" t="inlineStr"/>
+      <c r="AG36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5139,6 +5819,23 @@
       <c r="AC37" t="n">
         <v>16</v>
       </c>
+      <c r="AD37" t="inlineStr">
+        <is>
+          <t>Stroke</t>
+        </is>
+      </c>
+      <c r="AE37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Chronic pain</t>
+        </is>
+      </c>
+      <c r="AF37" t="inlineStr"/>
+      <c r="AG37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5266,6 +5963,31 @@
       <c r="AC38" t="n">
         <v>10</v>
       </c>
+      <c r="AD38" t="inlineStr">
+        <is>
+          <t>Chronic pain</t>
+        </is>
+      </c>
+      <c r="AE38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Stroke</t>
+        </is>
+      </c>
+      <c r="AF38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Heart disease</t>
+        </is>
+      </c>
+      <c r="AG38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5393,6 +6115,27 @@
       <c r="AC39" t="n">
         <v>16</v>
       </c>
+      <c r="AD39" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
+      <c r="AE39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thyroid problems</t>
+        </is>
+      </c>
+      <c r="AF39" t="inlineStr"/>
+      <c r="AG39" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5516,6 +6259,15 @@
       <c r="AC40" t="n">
         <v>17</v>
       </c>
+      <c r="AD40" t="inlineStr"/>
+      <c r="AE40" t="inlineStr"/>
+      <c r="AF40" t="inlineStr"/>
+      <c r="AG40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5643,6 +6395,27 @@
       <c r="AC41" t="n">
         <v>15</v>
       </c>
+      <c r="AD41" t="inlineStr">
+        <is>
+          <t>High blood pressure</t>
+        </is>
+      </c>
+      <c r="AE41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Heart disease</t>
+        </is>
+      </c>
+      <c r="AF41" t="inlineStr"/>
+      <c r="AG41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5770,6 +6543,19 @@
       <c r="AC42" t="n">
         <v>11</v>
       </c>
+      <c r="AD42" t="inlineStr">
+        <is>
+          <t>Cancer</t>
+        </is>
+      </c>
+      <c r="AE42" t="inlineStr"/>
+      <c r="AF42" t="inlineStr"/>
+      <c r="AG42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5897,6 +6683,27 @@
       <c r="AC43" t="n">
         <v>13</v>
       </c>
+      <c r="AD43" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="AE43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Chronic pain</t>
+        </is>
+      </c>
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Heart disease</t>
+        </is>
+      </c>
+      <c r="AG43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -6024,6 +6831,23 @@
       <c r="AC44" t="n">
         <v>13</v>
       </c>
+      <c r="AD44" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
+      <c r="AE44" t="inlineStr"/>
+      <c r="AF44" t="inlineStr"/>
+      <c r="AG44" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -6151,6 +6975,19 @@
       <c r="AC45" t="n">
         <v>11</v>
       </c>
+      <c r="AD45" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="AE45" t="inlineStr"/>
+      <c r="AF45" t="inlineStr"/>
+      <c r="AG45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -6278,6 +7115,19 @@
       <c r="AC46" t="n">
         <v>18</v>
       </c>
+      <c r="AD46" t="inlineStr">
+        <is>
+          <t>Diabetes</t>
+        </is>
+      </c>
+      <c r="AE46" t="inlineStr"/>
+      <c r="AF46" t="inlineStr"/>
+      <c r="AG46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6405,6 +7255,19 @@
       <c r="AC47" t="n">
         <v>16</v>
       </c>
+      <c r="AD47" t="inlineStr">
+        <is>
+          <t>Thyroid problems</t>
+        </is>
+      </c>
+      <c r="AE47" t="inlineStr"/>
+      <c r="AF47" t="inlineStr"/>
+      <c r="AG47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6532,6 +7395,23 @@
       <c r="AC48" t="n">
         <v>11</v>
       </c>
+      <c r="AD48" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
+      <c r="AE48" t="inlineStr"/>
+      <c r="AF48" t="inlineStr"/>
+      <c r="AG48" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -6659,6 +7539,31 @@
       <c r="AC49" t="n">
         <v>11</v>
       </c>
+      <c r="AD49" t="inlineStr">
+        <is>
+          <t>Thyroid problems</t>
+        </is>
+      </c>
+      <c r="AE49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AF49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Heart disease</t>
+        </is>
+      </c>
+      <c r="AG49" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -6782,6 +7687,15 @@
       <c r="AC50" t="n">
         <v>14</v>
       </c>
+      <c r="AD50" t="inlineStr"/>
+      <c r="AE50" t="inlineStr"/>
+      <c r="AF50" t="inlineStr"/>
+      <c r="AG50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -6909,6 +7823,31 @@
       <c r="AC51" t="n">
         <v>12</v>
       </c>
+      <c r="AD51" t="inlineStr">
+        <is>
+          <t>Thyroid problems</t>
+        </is>
+      </c>
+      <c r="AE51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Cancer</t>
+        </is>
+      </c>
+      <c r="AF51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> None</t>
+        </is>
+      </c>
+      <c r="AG51" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -7036,6 +7975,19 @@
       <c r="AC52" t="n">
         <v>12</v>
       </c>
+      <c r="AD52" t="inlineStr">
+        <is>
+          <t>Thyroid problems</t>
+        </is>
+      </c>
+      <c r="AE52" t="inlineStr"/>
+      <c r="AF52" t="inlineStr"/>
+      <c r="AG52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -7163,6 +8115,19 @@
       <c r="AC53" t="n">
         <v>13</v>
       </c>
+      <c r="AD53" t="inlineStr">
+        <is>
+          <t>Stroke</t>
+        </is>
+      </c>
+      <c r="AE53" t="inlineStr"/>
+      <c r="AF53" t="inlineStr"/>
+      <c r="AG53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -7290,6 +8255,27 @@
       <c r="AC54" t="n">
         <v>14</v>
       </c>
+      <c r="AD54" t="inlineStr">
+        <is>
+          <t>Stroke</t>
+        </is>
+      </c>
+      <c r="AE54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AF54" t="inlineStr"/>
+      <c r="AG54" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -7417,6 +8403,31 @@
       <c r="AC55" t="n">
         <v>6</v>
       </c>
+      <c r="AD55" t="inlineStr">
+        <is>
+          <t>Thyroid problems</t>
+        </is>
+      </c>
+      <c r="AE55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AF55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Cancer</t>
+        </is>
+      </c>
+      <c r="AG55" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -7544,6 +8555,31 @@
       <c r="AC56" t="n">
         <v>9</v>
       </c>
+      <c r="AD56" t="inlineStr">
+        <is>
+          <t>Cancer</t>
+        </is>
+      </c>
+      <c r="AE56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Stroke</t>
+        </is>
+      </c>
+      <c r="AF56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Neurological disorders</t>
+        </is>
+      </c>
+      <c r="AG56" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> several</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -7671,6 +8707,19 @@
       <c r="AC57" t="n">
         <v>12</v>
       </c>
+      <c r="AD57" t="inlineStr">
+        <is>
+          <t>Neurological disorders</t>
+        </is>
+      </c>
+      <c r="AE57" t="inlineStr"/>
+      <c r="AF57" t="inlineStr"/>
+      <c r="AG57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -7798,6 +8847,27 @@
       <c r="AC58" t="n">
         <v>12</v>
       </c>
+      <c r="AD58" t="inlineStr">
+        <is>
+          <t>Stroke</t>
+        </is>
+      </c>
+      <c r="AE58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> None</t>
+        </is>
+      </c>
+      <c r="AF58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AG58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -7925,6 +8995,27 @@
       <c r="AC59" t="n">
         <v>15</v>
       </c>
+      <c r="AD59" t="inlineStr">
+        <is>
+          <t>Stroke</t>
+        </is>
+      </c>
+      <c r="AE59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> High blood pressure</t>
+        </is>
+      </c>
+      <c r="AF59" t="inlineStr"/>
+      <c r="AG59" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -8052,6 +9143,19 @@
       <c r="AC60" t="n">
         <v>17</v>
       </c>
+      <c r="AD60" t="inlineStr">
+        <is>
+          <t>Diabetes</t>
+        </is>
+      </c>
+      <c r="AE60" t="inlineStr"/>
+      <c r="AF60" t="inlineStr"/>
+      <c r="AG60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AH60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -8178,6 +9282,23 @@
       </c>
       <c r="AC61" t="n">
         <v>13</v>
+      </c>
+      <c r="AD61" t="inlineStr">
+        <is>
+          <t>Neurological disorders</t>
+        </is>
+      </c>
+      <c r="AE61" t="inlineStr"/>
+      <c r="AF61" t="inlineStr"/>
+      <c r="AG61" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AH61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> one or two</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preprocesasing  and edit profile bug fixed
</commit_message>
<xml_diff>
--- a/BSDT-statistical-analysis/media/ID_36_uploads/temporary_uploads/Depression_Questionnaire_Responses.xlsx
+++ b/BSDT-statistical-analysis/media/ID_36_uploads/temporary_uploads/Depression_Questionnaire_Responses.xlsx
@@ -2801,7 +2801,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
       <c r="O19" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -4956,7 +4960,11 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="N36" t="inlineStr"/>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
       <c r="O36" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -5460,7 +5468,11 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="N40" t="inlineStr"/>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
       <c r="O40" t="inlineStr">
         <is>
           <t>No</t>
@@ -6726,7 +6738,11 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="N50" t="inlineStr"/>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>Heart disease</t>
+        </is>
+      </c>
       <c r="O50" t="inlineStr">
         <is>
           <t>Yes</t>

</xml_diff>